<commit_message>
Refactor available_options.json to consolidate service definitions and update blueprint_services configuration for enhanced data validation. Modify transformation logic to include new service mappings for improved processing accuracy.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_services.xlsx
+++ b/input_tables/blueprint_services.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
   <si>
     <t xml:space="preserve">Service</t>
   </si>
@@ -38,6 +38,231 @@
   </si>
   <si>
     <t xml:space="preserve">enhancement medium specification (enhancement:taskProduct)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pano Blurring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blur: Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pano Retouching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo-enhancement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo-enhancement: Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pano Decluttering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declutter: Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pano Staging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staging: Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floorplan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry-scaffold-building: IM-operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry-scaffold:Geometry-building-spins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLA Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry-scaffold-building: auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto GLA Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Material Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiDAR Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiDAR GLA Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiDAR Material Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto LiDAR Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto LiDAR GLA Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto LiDAR Material Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RoomPlan Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry-building: IM-operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometry-scaffold:Geometry-building-roomPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RoomPlan GLA Floor Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor Measurements &amp; Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor-measurements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walls, Floors, Ceilings &amp; Wall Element Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walls-and-wall-elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Elevation Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkthrough-tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blurred Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retouched Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decluttered Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staged Walkthrough Tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement-tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermo-view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flythrough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkthrough Video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkthrough-video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dollhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Dollhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR Photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hdr-images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo Capture: IM-operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panos:Pano-Generation-spins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto HDR Photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo Capture: auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR Photo Blurring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blurring: Panos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR Photo Retouching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo enhancement: Hdr-images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR Photo Decluttering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR Photo Staging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curbshot Photo Retouching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSLR Photos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panos:Pano-Generation-dslr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSLR Photo Retouching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSLR Photo Decluttering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Declutter: Hdr-images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSLR Photo Staging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staging: Hdr-images</t>
   </si>
 </sst>
 </file>
@@ -142,12 +367,12 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="A2:F24"/>
+      <selection pane="bottomLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>
@@ -181,73 +406,616 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="I20" s="1"/>
     </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="I35" s="1"/>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="I52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="I53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="I54" s="1"/>
     </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="I59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>78</v>
+      </c>
       <c r="I60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>80</v>
+      </c>
       <c r="I61" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor available_options.json to remove deprecated task and service definitions, enhancing data validation logic. Update transformation functions to incorporate new task relationships and validation checks for specification fields, improving data integrity and processing accuracy.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_services.xlsx
+++ b/input_tables/blueprint_services.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="80">
   <si>
     <t xml:space="preserve">Service</t>
   </si>
@@ -85,7 +85,25 @@
     <t xml:space="preserve">Floorplan</t>
   </si>
   <si>
-    <t xml:space="preserve">geometry-scaffold-building: IM-operators</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Geometry-building-spins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: IM-operators</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">geometry-scaffold:Geometry-building-spins</t>
@@ -100,7 +118,25 @@
     <t xml:space="preserve">Auto Floor Plan</t>
   </si>
   <si>
-    <t xml:space="preserve">geometry-scaffold-building: auto</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Geometry-building-spins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: auto</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Auto GLA Floor Plan</t>
@@ -130,7 +166,25 @@
     <t xml:space="preserve">RoomPlan Floor Plan</t>
   </si>
   <si>
-    <t xml:space="preserve">geometry-building: IM-operators</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Geometry-building-roomPlan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: IM-operators</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">geometry-scaffold:Geometry-building-roomPlan</t>
@@ -211,7 +265,7 @@
     <t xml:space="preserve">Hdr-images</t>
   </si>
   <si>
-    <t xml:space="preserve">Photo Capture: IM-operators</t>
+    <t xml:space="preserve">Photo-Capture: IM-operators</t>
   </si>
   <si>
     <t xml:space="preserve">Panos:Pano-Generation-spins</t>
@@ -220,19 +274,16 @@
     <t xml:space="preserve">Auto HDR Photos</t>
   </si>
   <si>
-    <t xml:space="preserve">Photo Capture: auto</t>
+    <t xml:space="preserve">Photo-Capture: auto</t>
   </si>
   <si>
     <t xml:space="preserve">HDR Photo Blurring</t>
   </si>
   <si>
-    <t xml:space="preserve">Blurring: Panos</t>
-  </si>
-  <si>
     <t xml:space="preserve">HDR Photo Retouching</t>
   </si>
   <si>
-    <t xml:space="preserve">Photo enhancement: Hdr-images</t>
+    <t xml:space="preserve">Photo-enhancement: Hdr-images</t>
   </si>
   <si>
     <t xml:space="preserve">HDR Photo Decluttering</t>
@@ -272,7 +323,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -292,6 +343,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -338,8 +395,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,12 +428,12 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>
@@ -469,13 +530,13 @@
       <c r="B8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -484,13 +545,13 @@
       <c r="B9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -499,13 +560,13 @@
       <c r="B10" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -514,13 +575,13 @@
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -529,13 +590,13 @@
       <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -544,13 +605,13 @@
       <c r="B13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -559,13 +620,13 @@
       <c r="B15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -574,13 +635,13 @@
       <c r="B16" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -589,13 +650,13 @@
       <c r="B17" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -604,13 +665,13 @@
       <c r="B18" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -619,13 +680,13 @@
       <c r="B19" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -634,13 +695,13 @@
       <c r="B20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -649,7 +710,7 @@
       <c r="B22" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E22" s="0" t="s">
@@ -663,7 +724,7 @@
       <c r="B23" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="0" t="s">
@@ -701,8 +762,8 @@
       <c r="B30" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>36</v>
+      <c r="D30" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +773,7 @@
       <c r="B31" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -726,10 +787,10 @@
       <c r="C32" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -741,10 +802,10 @@
       <c r="C33" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -756,10 +817,10 @@
       <c r="C34" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -771,10 +832,10 @@
       <c r="C35" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -815,8 +876,8 @@
       <c r="B45" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>36</v>
+      <c r="D45" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,7 +887,7 @@
       <c r="B46" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -875,13 +936,13 @@
         <v>64</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I51" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="I51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>62</v>
@@ -896,13 +957,13 @@
         <v>64</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I52" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>62</v>
@@ -919,11 +980,11 @@
       <c r="F53" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="1"/>
+      <c r="I53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>62</v>
@@ -934,11 +995,11 @@
       <c r="E54" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="I54" s="1"/>
+      <c r="I54" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>62</v>
@@ -950,23 +1011,23 @@
         <v>64</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>62</v>
@@ -975,16 +1036,16 @@
         <v>11</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="I59" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="I59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>62</v>
@@ -993,16 +1054,16 @@
         <v>14</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I60" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="I60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>62</v>
@@ -1011,12 +1072,12 @@
         <v>17</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I61" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="I61" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Update blueprint_services.xlsx to reflect recent changes in task and service definitions, enhancing data organization and validation consistency.
</commit_message>
<xml_diff>
--- a/input_tables/blueprint_services.xlsx
+++ b/input_tables/blueprint_services.xlsx
@@ -85,25 +85,7 @@
     <t xml:space="preserve">Floorplan</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Geometry-building-spins</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: IM-operators</t>
-    </r>
+    <t xml:space="preserve">Geometry-building-spins: IM-operators</t>
   </si>
   <si>
     <t xml:space="preserve">geometry-scaffold:Geometry-building-spins</t>
@@ -118,25 +100,7 @@
     <t xml:space="preserve">Auto Floor Plan</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Geometry-building-spins</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: auto</t>
-    </r>
+    <t xml:space="preserve">Geometry-building-spins: auto</t>
   </si>
   <si>
     <t xml:space="preserve">Auto GLA Floor Plan</t>
@@ -166,25 +130,7 @@
     <t xml:space="preserve">RoomPlan Floor Plan</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Geometry-building-roomPlan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">: IM-operators</t>
-    </r>
+    <t xml:space="preserve">Geometry-building-roomPlan: IM-operators</t>
   </si>
   <si>
     <t xml:space="preserve">geometry-scaffold:Geometry-building-roomPlan</t>
@@ -323,7 +269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -343,12 +289,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -400,7 +340,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -430,10 +370,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+      <selection pane="bottomLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>

</xml_diff>